<commit_message>
Add Jiménez 2019 pattern generator and evaluation functions
</commit_message>
<xml_diff>
--- a/compared/compare_results.xlsx
+++ b/compared/compare_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -474,7 +474,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, o2008, d2006</t>
+          <t>o1980, o1988, o1992b, o2008</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ATATTAATAT</t>
+          <t>ATATATTAAT</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -512,7 +512,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TAATATATAT</t>
+          <t>ATATATAAAT</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -520,7 +520,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, o2008, d2006</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ATATAAATAT</t>
+          <t>ATATTAATAT</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -543,7 +543,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b</t>
+          <t>o1980, o1988, o2008</t>
         </is>
       </c>
     </row>
@@ -558,7 +558,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ATATATTAAT</t>
+          <t>TAATATATAT</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>o1980, o1988, o2008</t>
+          <t>o1980, o1988, o1992b, o2008</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ATATATAAAT</t>
+          <t>ATAAATATAT</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -589,7 +589,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -612,7 +612,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ATTAATATAT</t>
+          <t>ATATAAATAT</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -635,7 +635,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>o1980, o1988, o2008</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ATAAATATAT</t>
+          <t>ATTAATATAT</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -658,7 +658,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o1980, o1988, o2008</t>
         </is>
       </c>
     </row>
@@ -673,7 +673,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ATTAAAATAT</t>
+          <t>ATAAATAAAT</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -681,7 +681,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -696,7 +696,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>AAATATTAAT</t>
+          <t>AAAAATATAT</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -704,7 +704,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>o1980, o1988</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>AATAATATAT</t>
+          <t>AAATATAAAT</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -727,7 +727,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, o2008</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -737,12 +737,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ATATTATAAT</t>
+          <t>AAATTAATAT</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -750,7 +750,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980, o1988</t>
         </is>
       </c>
     </row>
@@ -760,12 +760,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>o1988</t>
+          <t>o1980</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ATTAATAAAT</t>
+          <t>TAATAAATAT</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -773,7 +773,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>o1988</t>
+          <t>o1980, o1992b</t>
         </is>
       </c>
     </row>
@@ -783,12 +783,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>TAATATTAAT</t>
+          <t>AATAATATAT</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -796,7 +796,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980, o1988, o1992b, o2008</t>
         </is>
       </c>
     </row>
@@ -806,12 +806,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ATTAATTAAT</t>
+          <t>ATTAAAATAT</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -819,7 +819,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980</t>
         </is>
       </c>
     </row>
@@ -842,7 +842,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -852,12 +852,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>TAATTAATAT</t>
+          <t>ATATAATAAT</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -865,7 +865,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980, o1988, o1992b, o2008</t>
         </is>
       </c>
     </row>
@@ -880,7 +880,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>AAATATAAAT</t>
+          <t>TAATATAAAT</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -888,7 +888,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -903,7 +903,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>AAATAAATAT</t>
+          <t>ATAATAATAT</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b</t>
+          <t>o1980, o1988</t>
         </is>
       </c>
     </row>
@@ -926,7 +926,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TAATAAATAT</t>
+          <t>AAATATTAAT</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -934,7 +934,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>o1980, o1992b</t>
+          <t>o1980, o1988</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ATAAAAATAT</t>
+          <t>ATATAAAAAT</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -957,7 +957,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>o1980, o1988</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -972,7 +972,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ATAATAATAT</t>
+          <t>ATAAATTAAT</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -980,7 +980,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>o1980, o1988</t>
+          <t>o1980</t>
         </is>
       </c>
     </row>
@@ -995,7 +995,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ATATAAAAAT</t>
+          <t>ATAAAAATAT</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b</t>
+          <t>o1980, o1988</t>
         </is>
       </c>
     </row>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ATAAATTAAT</t>
+          <t>AAATAAATAT</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o2008</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>AAAAATATAT</t>
+          <t>TAATTAATAT</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o2008</t>
         </is>
       </c>
     </row>
@@ -1059,12 +1059,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o2008</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>AAATTAATAT</t>
+          <t>TAATATTAAT</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>o1980, o1988</t>
+          <t>o2008</t>
         </is>
       </c>
     </row>
@@ -1082,12 +1082,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o1988</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ATATAATAAT</t>
+          <t>ATTAATAAAT</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, o2008</t>
+          <t>o1988</t>
         </is>
       </c>
     </row>
@@ -1105,12 +1105,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o2008</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>TAATATAAAT</t>
+          <t>ATTAATTAAT</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o2008</t>
         </is>
       </c>
     </row>
@@ -1128,12 +1128,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o2008</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ATAAATAAAT</t>
+          <t>ATATTATAAT</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o2008</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>AAAAATTAAT</t>
+          <t>ATAAAATAAT</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1174,12 +1174,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>TAATTATAAT</t>
+          <t>AAATAAAAAT</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -1197,12 +1197,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>AATAATTAAT</t>
+          <t>AAATAATAAT</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>o2008</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -1220,12 +1220,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>o1988</t>
+          <t>o1980</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>AATAATAAAT</t>
+          <t>AATAAAATAT</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>o1988, o1992b</t>
+          <t>o1980</t>
         </is>
       </c>
     </row>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TAAAAAATAT</t>
+          <t>AAAAATAAAT</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>AAAAAAATAT</t>
+          <t>AAAAATTAAT</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>o1980, o1988</t>
+          <t>o1980</t>
         </is>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TAATAAAAAT</t>
+          <t>ATAAAAAAAT</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1302,7 +1302,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>o1980, o1992b</t>
+          <t>o1980, o1988</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TAAAATAAAT</t>
+          <t>TAAAAAATAT</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o1980</t>
         </is>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>AAATAAAAAT</t>
+          <t>AAAATAATAT</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b</t>
+          <t>o1980, o1988</t>
         </is>
       </c>
     </row>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>AAAAATAAAT</t>
+          <t>AAAAAAATAT</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b, d2006</t>
+          <t>o1980, o1988</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ATAAAATAAT</t>
+          <t>TAATAAAAAT</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o1980, o1992b</t>
         </is>
       </c>
     </row>
@@ -1404,12 +1404,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o1988</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>AAAATAATAT</t>
+          <t>AATAATAAAT</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>o1980, o1988</t>
+          <t>o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>AATAAAATAT</t>
+          <t>TAAAATAAAT</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1440,7 +1440,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o1980, o1988, o1992b</t>
         </is>
       </c>
     </row>
@@ -1450,12 +1450,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o2008</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ATAAAAAAAT</t>
+          <t>TAATAATAAT</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>o1980, o1988</t>
+          <t>o2008</t>
         </is>
       </c>
     </row>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>TAATAATAAT</t>
+          <t>TATAATTAAT</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1496,12 +1496,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>o1980</t>
+          <t>o2008</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>AAATAATAAT</t>
+          <t>TAATTATAAT</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>o1980, o1988, o1992b</t>
+          <t>o2008</t>
         </is>
       </c>
     </row>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>TATAATTAAT</t>
+          <t>AATAATTAAT</t>
         </is>
       </c>
       <c r="D48" t="n">

</xml_diff>